<commit_message>
functions in spark added
</commit_message>
<xml_diff>
--- a/MBRDNA/Driving_events.xlsx
+++ b/MBRDNA/Driving_events.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabi/Dev/projects/MBRDNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{155E059D-6FCD-7E4D-9DA0-212C96FB7CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F30227E-E33A-4A47-AFEA-B1CB1FD79FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{6B17267D-C561-AE47-889C-050CC665ECFF}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6B17267D-C561-AE47-889C-050CC665ECFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Time</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>aux_off</t>
-  </si>
-  <si>
-    <t>windo_open</t>
   </si>
   <si>
     <t>end_drive</t>
@@ -421,7 +418,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +436,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -575,10 +572,6 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="str">
-        <f>+B2</f>
-        <v>start_drive</v>
-      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -671,7 +664,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -770,7 +763,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>